<commit_message>
feat : ajoute un test pour s'assurer que le user configuré existe dans le fichier excel
</commit_message>
<xml_diff>
--- a/test/resources/initialisation/userBase.xlsx
+++ b/test/resources/initialisation/userBase.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="183">
   <si>
     <t xml:space="preserve">NIVEAU HABILITATION</t>
   </si>
@@ -134,6 +134,36 @@
     <t xml:space="preserve">kcadmin</t>
   </si>
   <si>
+    <t xml:space="preserve">ti_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOTHER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un mec pas de l’URSSAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quelqun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pasdelurssaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quelqun@pasdelurssaf.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pasdelurssaf.fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGION</t>
   </si>
   <si>
@@ -414,9 +444,6 @@
   </si>
   <si>
     <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
   </si>
   <si>
     <t xml:space="preserve">78</t>
@@ -718,17 +745,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
@@ -736,6 +763,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +907,7 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -890,10 +918,43 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K1145"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="john.doe@zone51.gov.fr"/>
+    <hyperlink ref="H5" r:id="rId2" display="quelqun@pasdelurssaf.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -902,7 +963,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -917,7 +978,7 @@
       <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.36"/>
@@ -926,65 +987,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>16</v>
@@ -992,1058 +1053,1058 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
demande une confirmation à l'utilisateur s'il y a trop de changements au niveau des users (#8)
* feat : ajoute un test pour s'assurer que le user configuré existe dans le fichier excel

* feat : prepare la méthode pour demander au user de valider les changements s'il y en a trop

* feat : demande une confirmation à l'utilisateur s'il y a + de 10 modifications utilisateurs

Co-authored-by: Raphaël Squelbut <raphael.squelbut@alibeez.com>
</commit_message>
<xml_diff>
--- a/test/resources/initialisation/userBase.xlsx
+++ b/test/resources/initialisation/userBase.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="183">
   <si>
     <t xml:space="preserve">NIVEAU HABILITATION</t>
   </si>
@@ -134,6 +134,36 @@
     <t xml:space="preserve">kcadmin</t>
   </si>
   <si>
+    <t xml:space="preserve">ti_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANOTHER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un mec pas de l’URSSAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quelqun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pasdelurssaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quelqun@pasdelurssaf.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pasdelurssaf.fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGION</t>
   </si>
   <si>
@@ -414,9 +444,6 @@
   </si>
   <si>
     <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
   </si>
   <si>
     <t xml:space="preserve">78</t>
@@ -718,17 +745,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
@@ -736,6 +763,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +907,7 @@
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -890,10 +918,43 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K1145"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="john.doe@zone51.gov.fr"/>
+    <hyperlink ref="H5" r:id="rId2" display="quelqun@pasdelurssaf.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -902,7 +963,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -917,7 +978,7 @@
       <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.36"/>
@@ -926,65 +987,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>16</v>
@@ -992,1058 +1053,1058 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>